<commit_message>
actualizada demanda en el 2021
</commit_message>
<xml_diff>
--- a/DemandaUPME.xlsx
+++ b/DemandaUPME.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanl\Desktop\Desarrollos PHC\documents_to_consult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD3DA6E-32EB-4DEE-A107-CA4348789B8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAE2981-92E1-4283-8B93-A619A6A8B0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DemandaUPME" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -50,6 +51,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -535,9 +539,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -896,7 +902,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,351 +942,365 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2019</v>
-      </c>
-      <c r="B3">
-        <v>10882.59</v>
-      </c>
-      <c r="C3">
-        <v>10640.56</v>
-      </c>
-      <c r="D3">
-        <v>10640.56</v>
-      </c>
-      <c r="E3">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="F3">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="G3">
-        <v>4.3999999999999997E-2</v>
+        <v>2021</v>
+      </c>
+      <c r="B3" s="3">
+        <v>11184.005964552396</v>
+      </c>
+      <c r="C3" s="3">
+        <v>10800.560666229925</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10430.642935104692</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7.2073101519286809E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3.5316916701567669E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-1.4254662233958992E-4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2020</v>
-      </c>
-      <c r="B4">
-        <v>11113.004000000001</v>
-      </c>
-      <c r="C4">
-        <v>10764</v>
-      </c>
-      <c r="D4">
-        <v>10426.304</v>
-      </c>
-      <c r="E4">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="F4">
-        <v>1.2E-2</v>
-      </c>
-      <c r="G4">
-        <v>-0.02</v>
+        <v>2022</v>
+      </c>
+      <c r="B4" s="3">
+        <v>11485.919550478437</v>
+      </c>
+      <c r="C4" s="3">
+        <v>11095.821489423099</v>
+      </c>
+      <c r="D4" s="3">
+        <v>10719.485698390434</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.6995120253239469E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2.7337545921700679E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2.7691750650732372E-2</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2021</v>
-      </c>
-      <c r="B5">
-        <v>11401.514999999999</v>
-      </c>
-      <c r="C5">
-        <v>11047</v>
-      </c>
-      <c r="D5">
-        <v>10703.958000000001</v>
-      </c>
-      <c r="E5">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="F5">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="G5">
-        <v>2.7E-2</v>
+        <v>2023</v>
+      </c>
+      <c r="B5" s="3">
+        <v>11738.59388215597</v>
+      </c>
+      <c r="C5" s="3">
+        <v>11343.464488110016</v>
+      </c>
+      <c r="D5" s="3">
+        <v>10962.274864490102</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.199861583280982E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.2318581722225561E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2.2649329728209322E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2022</v>
-      </c>
-      <c r="B6">
-        <v>11692.541999999999</v>
-      </c>
-      <c r="C6">
-        <v>11331</v>
-      </c>
-      <c r="D6">
-        <v>10981.173000000001</v>
-      </c>
-      <c r="E6">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="F6">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="G6">
-        <v>2.5999999999999999E-2</v>
+        <v>2024</v>
+      </c>
+      <c r="B6" s="3">
+        <v>11971.908450201006</v>
+      </c>
+      <c r="C6" s="3">
+        <v>11571.370878990316</v>
+      </c>
+      <c r="D6" s="3">
+        <v>11184.963873295164</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.9875853137717003E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.0091427193093203E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2.0314123807131823E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2023</v>
-      </c>
-      <c r="B7">
-        <v>11969.921</v>
-      </c>
-      <c r="C7">
-        <v>11601</v>
-      </c>
-      <c r="D7">
-        <v>11244.022999999999</v>
-      </c>
-      <c r="E7">
-        <v>2.4E-2</v>
-      </c>
-      <c r="F7">
-        <v>2.4E-2</v>
-      </c>
-      <c r="G7">
-        <v>2.4E-2</v>
+        <v>2025</v>
+      </c>
+      <c r="B7" s="3">
+        <v>12196.22872010577</v>
+      </c>
+      <c r="C7" s="3">
+        <v>11790.809844707024</v>
+      </c>
+      <c r="D7" s="3">
+        <v>11399.69374236086</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.8737218952004087E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.8963955784628395E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.9198083382135689E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2024</v>
-      </c>
-      <c r="B8">
-        <v>12168.331</v>
-      </c>
-      <c r="C8">
-        <v>11804</v>
-      </c>
-      <c r="D8">
-        <v>11451.458000000001</v>
-      </c>
-      <c r="E8">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F8">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="G8">
-        <v>1.7999999999999999E-2</v>
+        <v>2026</v>
+      </c>
+      <c r="B8" s="3">
+        <v>12393.361055697593</v>
+      </c>
+      <c r="C8" s="3">
+        <v>11980.098848455047</v>
+      </c>
+      <c r="D8" s="3">
+        <v>11581.41611917979</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.6163384609772402E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.605394423632367E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.5940987620014502E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2025</v>
-      </c>
-      <c r="B9">
-        <v>12375.688</v>
-      </c>
-      <c r="C9">
-        <v>12003</v>
-      </c>
-      <c r="D9">
-        <v>11642.392</v>
-      </c>
-      <c r="E9">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F9">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="G9">
-        <v>1.7000000000000001E-2</v>
+        <v>2027</v>
+      </c>
+      <c r="B9" s="3">
+        <v>12528.194017831041</v>
+      </c>
+      <c r="C9" s="3">
+        <v>12109.522925620086</v>
+      </c>
+      <c r="D9" s="3">
+        <v>11705.622131436523</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.0879450822701697E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.0803256200321742E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.0724596282404297E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2026</v>
-      </c>
-      <c r="B10">
-        <v>12531.849</v>
-      </c>
-      <c r="C10">
-        <v>12152</v>
-      </c>
-      <c r="D10">
-        <v>11784.457</v>
-      </c>
-      <c r="E10">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="F10">
-        <v>1.2E-2</v>
-      </c>
-      <c r="G10">
-        <v>1.2E-2</v>
+        <v>2028</v>
+      </c>
+      <c r="B10" s="3">
+        <v>12756.818281335187</v>
+      </c>
+      <c r="C10" s="3">
+        <v>12333.404921088413</v>
+      </c>
+      <c r="D10" s="3">
+        <v>11924.929161349472</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.8248780564760647E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.8488093779042369E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.8735187882409132E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2027</v>
-      </c>
-      <c r="B11">
-        <v>12668.5</v>
-      </c>
-      <c r="C11">
-        <v>12282.735000000001</v>
-      </c>
-      <c r="D11">
-        <v>11909.455</v>
-      </c>
-      <c r="E11">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F11">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="G11">
-        <v>1.0999999999999999E-2</v>
+        <v>2029</v>
+      </c>
+      <c r="B11" s="3">
+        <v>12892.916661112198</v>
+      </c>
+      <c r="C11" s="3">
+        <v>12464.799265034775</v>
+      </c>
+      <c r="D11" s="3">
+        <v>12051.785423151601</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.0668677469219734E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.0653533617605904E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.0637904853413316E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2028</v>
-      </c>
-      <c r="B12">
-        <v>12814.513999999999</v>
-      </c>
-      <c r="C12">
-        <v>12423.974</v>
-      </c>
-      <c r="D12">
-        <v>12046.085999999999</v>
-      </c>
-      <c r="E12">
-        <v>1.2E-2</v>
-      </c>
-      <c r="F12">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="G12">
-        <v>1.0999999999999999E-2</v>
+        <v>2030</v>
+      </c>
+      <c r="B12" s="3">
+        <v>13043.571876154809</v>
+      </c>
+      <c r="C12" s="3">
+        <v>12610.619551866052</v>
+      </c>
+      <c r="D12" s="3">
+        <v>12192.941353210443</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.1685115090910303E-2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.1698566798449717E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1.1712449658096258E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2029</v>
-      </c>
-      <c r="B13">
-        <v>13021.17</v>
-      </c>
-      <c r="C13">
-        <v>12625.031000000001</v>
-      </c>
-      <c r="D13">
-        <v>12241.733</v>
-      </c>
-      <c r="E13">
-        <v>1.6E-2</v>
-      </c>
-      <c r="F13">
-        <v>1.6E-2</v>
-      </c>
-      <c r="G13">
-        <v>1.6E-2</v>
+        <v>2031</v>
+      </c>
+      <c r="B13" s="3">
+        <v>13280.808607270706</v>
+      </c>
+      <c r="C13" s="3">
+        <v>12839.571664933937</v>
+      </c>
+      <c r="D13" s="3">
+        <v>12413.901121281617</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.8188018847014931E-2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.8155500776645628E-2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1.8121941348712811E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2030</v>
-      </c>
-      <c r="B14">
-        <v>13311.346</v>
-      </c>
-      <c r="C14">
-        <v>12910.023999999999</v>
-      </c>
-      <c r="D14">
-        <v>12521.703</v>
-      </c>
-      <c r="E14">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="F14">
-        <v>2.3E-2</v>
-      </c>
-      <c r="G14">
-        <v>2.3E-2</v>
+        <v>2032</v>
+      </c>
+      <c r="B14" s="3">
+        <v>13449.224541937388</v>
+      </c>
+      <c r="C14" s="3">
+        <v>13002.58516014495</v>
+      </c>
+      <c r="D14" s="3">
+        <v>12571.702769705811</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.2681150647294359E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.2696178616006248E-2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.271168884643914E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2031</v>
-      </c>
-      <c r="B15">
-        <v>13532.299000000001</v>
-      </c>
-      <c r="C15">
-        <v>13125.726000000001</v>
-      </c>
-      <c r="D15">
-        <v>12732.322</v>
-      </c>
-      <c r="E15">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F15">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="G15">
-        <v>1.7000000000000001E-2</v>
+        <v>2033</v>
+      </c>
+      <c r="B15" s="3">
+        <v>13608.720179969227</v>
+      </c>
+      <c r="C15" s="3">
+        <v>13156.831908902081</v>
+      </c>
+      <c r="D15" s="3">
+        <v>12720.885804760042</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.1859095484241466E-2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.1862775506360279E-2</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.186657350933551E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2032</v>
-      </c>
-      <c r="B16">
-        <v>13778.004999999999</v>
-      </c>
-      <c r="C16">
-        <v>13365.852999999999</v>
-      </c>
-      <c r="D16">
-        <v>12967.039000000001</v>
-      </c>
-      <c r="E16">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="F16">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="G16">
-        <v>1.7999999999999999E-2</v>
+        <v>2034</v>
+      </c>
+      <c r="B16" s="3">
+        <v>13767.669364347024</v>
+      </c>
+      <c r="C16" s="3">
+        <v>13310.451234886956</v>
+      </c>
+      <c r="D16" s="3">
+        <v>12869.363304433435</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.1679950963482622E-2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.1676011903818173E-2</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.1671946588643456E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2033</v>
-      </c>
-      <c r="B17">
-        <v>14056.885</v>
-      </c>
-      <c r="C17">
-        <v>13639.472</v>
-      </c>
-      <c r="D17">
-        <v>13235.584000000001</v>
-      </c>
-      <c r="E17">
-        <v>0.02</v>
-      </c>
-      <c r="F17">
-        <v>0.02</v>
-      </c>
-      <c r="G17">
-        <v>2.1000000000000001E-2</v>
+        <v>2035</v>
+      </c>
+      <c r="B17" s="3">
+        <v>13931.059217599754</v>
+      </c>
+      <c r="C17" s="3">
+        <v>13468.280158570407</v>
+      </c>
+      <c r="D17" s="3">
+        <v>13021.827482589393</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1.1867647960507099E-2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.1857518644430298E-2</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.1847064578823119E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04962302-36AC-43D2-915B-B8CE37B29C8F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
redondeado a 4 cifras
</commit_message>
<xml_diff>
--- a/DemandaUPME.xlsx
+++ b/DemandaUPME.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanl\Desktop\Desarrollos PHC\documents_to_consult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6677AAA8-E081-4752-B05B-4168DDFE7DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9899A671-0443-4B58-9FEA-BF08950EA954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -554,7 +554,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -913,7 +913,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:O1048576"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,19 +959,19 @@
         <v>11184.005999999999</v>
       </c>
       <c r="C3" s="2">
-        <v>10800.561</v>
+        <v>10800.5607</v>
       </c>
       <c r="D3" s="2">
-        <v>10430.643</v>
+        <v>10430.642900000001</v>
       </c>
       <c r="E3" s="2">
-        <v>7.1999999999999995E-2</v>
+        <v>7.2099999999999997E-2</v>
       </c>
       <c r="F3" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5299999999999998E-2</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>-1E-4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -979,22 +979,22 @@
         <v>2022</v>
       </c>
       <c r="B4" s="2">
-        <v>11485.92</v>
+        <v>11485.919599999999</v>
       </c>
       <c r="C4" s="2">
-        <v>11095.821</v>
+        <v>11095.8215</v>
       </c>
       <c r="D4" s="2">
-        <v>10719.486000000001</v>
+        <v>10719.485699999999</v>
       </c>
       <c r="E4" s="2">
         <v>2.7E-2</v>
       </c>
       <c r="F4" s="2">
-        <v>2.7E-2</v>
+        <v>2.7300000000000001E-2</v>
       </c>
       <c r="G4" s="2">
-        <v>2.8000000000000001E-2</v>
+        <v>2.7699999999999999E-2</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1003,22 +1003,22 @@
         <v>2023</v>
       </c>
       <c r="B5" s="2">
-        <v>11738.593999999999</v>
+        <v>11738.5939</v>
       </c>
       <c r="C5" s="2">
-        <v>11343.464</v>
+        <v>11343.4645</v>
       </c>
       <c r="D5" s="2">
-        <v>10962.275</v>
+        <v>10962.2749</v>
       </c>
       <c r="E5" s="2">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F5" s="2">
-        <v>2.1999999999999999E-2</v>
+        <v>2.23E-2</v>
       </c>
       <c r="G5" s="2">
-        <v>2.3E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1026,22 +1026,22 @@
         <v>2024</v>
       </c>
       <c r="B6" s="2">
-        <v>11971.907999999999</v>
+        <v>11971.9085</v>
       </c>
       <c r="C6" s="2">
-        <v>11571.370999999999</v>
+        <v>11571.3709</v>
       </c>
       <c r="D6" s="2">
-        <v>11184.964</v>
+        <v>11184.963900000001</v>
       </c>
       <c r="E6" s="2">
-        <v>0.02</v>
+        <v>1.9900000000000001E-2</v>
       </c>
       <c r="F6" s="2">
-        <v>0.02</v>
+        <v>2.01E-2</v>
       </c>
       <c r="G6" s="2">
-        <v>0.02</v>
+        <v>2.0299999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1049,22 +1049,22 @@
         <v>2025</v>
       </c>
       <c r="B7" s="2">
-        <v>12196.228999999999</v>
+        <v>12196.2287</v>
       </c>
       <c r="C7" s="2">
-        <v>11790.81</v>
+        <v>11790.809800000001</v>
       </c>
       <c r="D7" s="2">
-        <v>11399.694</v>
+        <v>11399.6937</v>
       </c>
       <c r="E7" s="2">
-        <v>1.9E-2</v>
+        <v>1.8700000000000001E-2</v>
       </c>
       <c r="F7" s="2">
         <v>1.9E-2</v>
       </c>
       <c r="G7" s="2">
-        <v>1.9E-2</v>
+        <v>1.9199999999999998E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1072,22 +1072,22 @@
         <v>2026</v>
       </c>
       <c r="B8" s="2">
-        <v>12393.361000000001</v>
+        <v>12393.3611</v>
       </c>
       <c r="C8" s="2">
-        <v>11980.099</v>
+        <v>11980.0988</v>
       </c>
       <c r="D8" s="2">
-        <v>11581.415999999999</v>
+        <v>11581.4161</v>
       </c>
       <c r="E8" s="2">
-        <v>1.6E-2</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="F8" s="2">
-        <v>1.6E-2</v>
+        <v>1.61E-2</v>
       </c>
       <c r="G8" s="2">
-        <v>1.6E-2</v>
+        <v>1.5900000000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1098,19 +1098,19 @@
         <v>12528.194</v>
       </c>
       <c r="C9" s="2">
-        <v>12109.522999999999</v>
+        <v>12109.5229</v>
       </c>
       <c r="D9" s="2">
-        <v>11705.621999999999</v>
+        <v>11705.622100000001</v>
       </c>
       <c r="E9" s="2">
-        <v>1.0999999999999999E-2</v>
+        <v>1.09E-2</v>
       </c>
       <c r="F9" s="2">
-        <v>1.0999999999999999E-2</v>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="G9" s="2">
-        <v>1.0999999999999999E-2</v>
+        <v>1.0699999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1118,22 +1118,22 @@
         <v>2028</v>
       </c>
       <c r="B10" s="2">
-        <v>12756.817999999999</v>
+        <v>12756.818300000001</v>
       </c>
       <c r="C10" s="2">
-        <v>12333.405000000001</v>
+        <v>12333.4049</v>
       </c>
       <c r="D10" s="2">
-        <v>11924.929</v>
+        <v>11924.9292</v>
       </c>
       <c r="E10" s="2">
-        <v>1.7999999999999999E-2</v>
+        <v>1.8200000000000001E-2</v>
       </c>
       <c r="F10" s="2">
-        <v>1.7999999999999999E-2</v>
+        <v>1.8499999999999999E-2</v>
       </c>
       <c r="G10" s="2">
-        <v>1.9E-2</v>
+        <v>1.8700000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1141,22 +1141,22 @@
         <v>2029</v>
       </c>
       <c r="B11" s="2">
-        <v>12892.916999999999</v>
+        <v>12892.9167</v>
       </c>
       <c r="C11" s="2">
-        <v>12464.799000000001</v>
+        <v>12464.799300000001</v>
       </c>
       <c r="D11" s="2">
-        <v>12051.785</v>
+        <v>12051.785400000001</v>
       </c>
       <c r="E11" s="2">
-        <v>1.0999999999999999E-2</v>
+        <v>1.0699999999999999E-2</v>
       </c>
       <c r="F11" s="2">
-        <v>1.0999999999999999E-2</v>
+        <v>1.0699999999999999E-2</v>
       </c>
       <c r="G11" s="2">
-        <v>1.0999999999999999E-2</v>
+        <v>1.06E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1164,22 +1164,22 @@
         <v>2030</v>
       </c>
       <c r="B12" s="2">
-        <v>13043.572</v>
+        <v>13043.571900000001</v>
       </c>
       <c r="C12" s="2">
-        <v>12610.62</v>
+        <v>12610.6196</v>
       </c>
       <c r="D12" s="2">
-        <v>12192.941000000001</v>
+        <v>12192.9414</v>
       </c>
       <c r="E12" s="2">
-        <v>1.2E-2</v>
+        <v>1.17E-2</v>
       </c>
       <c r="F12" s="2">
-        <v>1.2E-2</v>
+        <v>1.17E-2</v>
       </c>
       <c r="G12" s="2">
-        <v>1.2E-2</v>
+        <v>1.17E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1187,22 +1187,22 @@
         <v>2031</v>
       </c>
       <c r="B13" s="2">
-        <v>13280.808999999999</v>
+        <v>13280.8086</v>
       </c>
       <c r="C13" s="2">
-        <v>12839.572</v>
+        <v>12839.5717</v>
       </c>
       <c r="D13" s="2">
-        <v>12413.901</v>
+        <v>12413.901099999999</v>
       </c>
       <c r="E13" s="2">
-        <v>1.7999999999999999E-2</v>
+        <v>1.8200000000000001E-2</v>
       </c>
       <c r="F13" s="2">
-        <v>1.7999999999999999E-2</v>
+        <v>1.8200000000000001E-2</v>
       </c>
       <c r="G13" s="2">
-        <v>1.7999999999999999E-2</v>
+        <v>1.8100000000000002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1210,22 +1210,22 @@
         <v>2032</v>
       </c>
       <c r="B14" s="2">
-        <v>13449.225</v>
+        <v>13449.2245</v>
       </c>
       <c r="C14" s="2">
-        <v>13002.584999999999</v>
+        <v>13002.5852</v>
       </c>
       <c r="D14" s="2">
-        <v>12571.703</v>
+        <v>12571.702799999999</v>
       </c>
       <c r="E14" s="2">
-        <v>1.2999999999999999E-2</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="F14" s="2">
-        <v>1.2999999999999999E-2</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="G14" s="2">
-        <v>1.2999999999999999E-2</v>
+        <v>1.2699999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1233,22 +1233,22 @@
         <v>2033</v>
       </c>
       <c r="B15" s="2">
-        <v>13608.72</v>
+        <v>13608.7202</v>
       </c>
       <c r="C15" s="2">
-        <v>13156.832</v>
+        <v>13156.831899999999</v>
       </c>
       <c r="D15" s="2">
-        <v>12720.886</v>
+        <v>12720.8858</v>
       </c>
       <c r="E15" s="2">
-        <v>1.2E-2</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="F15" s="2">
-        <v>1.2E-2</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="G15" s="2">
-        <v>1.2E-2</v>
+        <v>1.1900000000000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1256,22 +1256,22 @@
         <v>2034</v>
       </c>
       <c r="B16" s="2">
-        <v>13767.669</v>
+        <v>13767.669400000001</v>
       </c>
       <c r="C16" s="2">
-        <v>13310.450999999999</v>
+        <v>13310.4512</v>
       </c>
       <c r="D16" s="2">
-        <v>12869.362999999999</v>
+        <v>12869.363300000001</v>
       </c>
       <c r="E16" s="2">
-        <v>1.2E-2</v>
+        <v>1.17E-2</v>
       </c>
       <c r="F16" s="2">
-        <v>1.2E-2</v>
+        <v>1.17E-2</v>
       </c>
       <c r="G16" s="2">
-        <v>1.2E-2</v>
+        <v>1.17E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1279,22 +1279,22 @@
         <v>2035</v>
       </c>
       <c r="B17" s="2">
-        <v>13931.058999999999</v>
+        <v>13931.0592</v>
       </c>
       <c r="C17" s="2">
-        <v>13468.28</v>
+        <v>13468.280199999999</v>
       </c>
       <c r="D17" s="2">
-        <v>13021.826999999999</v>
+        <v>13021.827499999999</v>
       </c>
       <c r="E17" s="2">
-        <v>1.2E-2</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="F17" s="2">
-        <v>1.2E-2</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="G17" s="2">
-        <v>1.2E-2</v>
+        <v>1.18E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>